<commit_message>
Exportacion de datos de las cargas de trabajo para proyecto de asiganaciones financieras
</commit_message>
<xml_diff>
--- a/src/output/cabanaconde_vigente.xlsx
+++ b/src/output/cabanaconde_vigente.xlsx
@@ -2403,55 +2403,55 @@
     </row>
     <row r="34" spans="2:21">
       <c r="I34" s="7">
-        <f>SUM(I12:I33)</f>
+        <f>SUM(I11:I33)</f>
         <v>0</v>
       </c>
       <c r="J34" s="7">
-        <f>SUM(J12:J33)</f>
+        <f>SUM(J11:J33)</f>
         <v>0</v>
       </c>
       <c r="K34" s="7">
-        <f>SUM(K12:K33)</f>
+        <f>SUM(K11:K33)</f>
         <v>0</v>
       </c>
       <c r="L34" s="7">
-        <f>SUM(L12:L33)</f>
+        <f>SUM(L11:L33)</f>
         <v>0</v>
       </c>
       <c r="M34" s="7">
-        <f>SUM(M12:M33)</f>
+        <f>SUM(M11:M33)</f>
         <v>0</v>
       </c>
       <c r="N34" s="7">
-        <f>SUM(N12:N33)</f>
+        <f>SUM(N11:N33)</f>
         <v>0</v>
       </c>
       <c r="O34" s="7">
-        <f>SUM(O12:O33)</f>
+        <f>SUM(O11:O33)</f>
         <v>0</v>
       </c>
       <c r="P34" s="7">
-        <f>SUM(P12:P33)</f>
+        <f>SUM(P11:P33)</f>
         <v>0</v>
       </c>
       <c r="Q34" s="7">
-        <f>SUM(Q12:Q33)</f>
+        <f>SUM(Q11:Q33)</f>
         <v>0</v>
       </c>
       <c r="R34" s="7">
-        <f>SUM(R12:R33)</f>
+        <f>SUM(R11:R33)</f>
         <v>0</v>
       </c>
       <c r="S34" s="7">
-        <f>SUM(S12:S33)</f>
+        <f>SUM(S11:S33)</f>
         <v>0</v>
       </c>
       <c r="T34" s="7">
-        <f>SUM(T12:T33)</f>
+        <f>SUM(T11:T33)</f>
         <v>0</v>
       </c>
       <c r="U34" s="7">
-        <f>SUM(U12:U33)</f>
+        <f>SUM(U11:U33)</f>
         <v>0</v>
       </c>
     </row>
@@ -3237,6 +3237,10 @@
       </c>
       <c r="E24" s="8" t="s">
         <v>61</v>
+      </c>
+      <c r="AJ24" s="7">
+        <f>SUM(F24:AI24)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:36">
@@ -4283,6 +4287,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AK24" s="7">
+        <f>SUM(F24:AJ24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8">
@@ -6155,6 +6163,8 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="40" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -6557,7 +6567,7 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A1:AF1"/>
     <mergeCell ref="A3:E4"/>
     <mergeCell ref="F3:J4"/>
     <mergeCell ref="K3:L4"/>
@@ -8026,6 +8036,10 @@
       </c>
       <c r="E24" s="8" t="s">
         <v>61</v>
+      </c>
+      <c r="AJ24" s="7">
+        <f>SUM(F24:AI24)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:36">
@@ -9120,6 +9134,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AK24" s="7">
+        <f>SUM(F24:AJ24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8">
@@ -10206,6 +10224,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AJ24" s="7">
+        <f>SUM(F24:AI24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:36">
       <c r="A25" s="8">
@@ -11314,6 +11336,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AK24" s="7">
+        <f>SUM(F24:AJ24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8">
@@ -12416,6 +12442,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AK24" s="7">
+        <f>SUM(F24:AJ24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8">
@@ -13502,6 +13532,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AJ24" s="7">
+        <f>SUM(F24:AI24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:36">
       <c r="A25" s="8">
@@ -14604,6 +14638,10 @@
       <c r="E24" s="8" t="s">
         <v>61</v>
       </c>
+      <c r="AK24" s="7">
+        <f>SUM(F24:AJ24)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="8">

</xml_diff>